<commit_message>
JS first 10 topics added in Technology Topics
</commit_message>
<xml_diff>
--- a/Angular Beginner.xlsx
+++ b/Angular Beginner.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bm46010926\Desktop\Mathar\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bm46010926\Desktop\unwanted\Mathar\Angular-9-Beginner-Tutorial\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="9735" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="9735"/>
   </bookViews>
   <sheets>
     <sheet name="Headings" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="100">
   <si>
     <t>Topic Headings:</t>
   </si>
@@ -527,6 +527,48 @@
   </si>
   <si>
     <t>2am - 2.30am</t>
+  </si>
+  <si>
+    <t>LifecycleHook - ( ngDoCheck, ngAfterViewInit)</t>
+  </si>
+  <si>
+    <t>LifeCycleHook - (ngAfterViewChecked to destory)</t>
+  </si>
+  <si>
+    <t>Template Reference variable, ngTemplate, ngContainer, ngtemplateOutet</t>
+  </si>
+  <si>
+    <t>@HostListener and Host binding</t>
+  </si>
+  <si>
+    <t>@Input, @Output, @Eventemitter</t>
+  </si>
+  <si>
+    <t>Pass data from parent to child | @Input decorator</t>
+  </si>
+  <si>
+    <t>Pass data from child to parent | @Output decorator</t>
+  </si>
+  <si>
+    <t>Pass data between slibings component | Observable</t>
+  </si>
+  <si>
+    <t>Observable</t>
+  </si>
+  <si>
+    <t>pipes | Inbuilt pipes | Custom pipes</t>
+  </si>
+  <si>
+    <t>Impure Pipe | Async Pipe</t>
+  </si>
+  <si>
+    <t>Routing &amp; Navigation</t>
+  </si>
+  <si>
+    <t>Service, Dependency Injection</t>
+  </si>
+  <si>
+    <t>HTTP service | curd operation</t>
   </si>
 </sst>
 </file>
@@ -939,10 +981,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J55"/>
+  <dimension ref="A1:L55"/>
   <sheetViews>
-    <sheetView topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="B29" sqref="B29"/>
+    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
+      <selection activeCell="C30" sqref="C30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1094,7 +1136,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="18.75">
+    <row r="17" spans="1:12" ht="18.75">
       <c r="B17" t="s">
         <v>38</v>
       </c>
@@ -1102,7 +1144,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="18" spans="1:7">
+    <row r="18" spans="1:12">
       <c r="B18" t="s">
         <v>16</v>
       </c>
@@ -1110,7 +1152,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="19" spans="1:7">
+    <row r="19" spans="1:12">
       <c r="B19" t="s">
         <v>17</v>
       </c>
@@ -1118,7 +1160,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="20" spans="1:7">
+    <row r="20" spans="1:12">
       <c r="B20" t="s">
         <v>18</v>
       </c>
@@ -1126,7 +1168,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="21" spans="1:7">
+    <row r="21" spans="1:12">
       <c r="A21">
         <v>6</v>
       </c>
@@ -1137,7 +1179,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="22" spans="1:7">
+    <row r="22" spans="1:12">
       <c r="B22" t="s">
         <v>22</v>
       </c>
@@ -1145,12 +1187,12 @@
         <v>74</v>
       </c>
     </row>
-    <row r="23" spans="1:7">
+    <row r="23" spans="1:12">
       <c r="B23" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="24" spans="1:7" ht="16.5">
+    <row r="24" spans="1:12" ht="16.5">
       <c r="B24" t="s">
         <v>39</v>
       </c>
@@ -1158,12 +1200,12 @@
         <v>21</v>
       </c>
     </row>
-    <row r="25" spans="1:7">
+    <row r="25" spans="1:12">
       <c r="B25" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="26" spans="1:7">
+    <row r="26" spans="1:12">
       <c r="B26" t="s">
         <v>24</v>
       </c>
@@ -1171,7 +1213,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="27" spans="1:7">
+    <row r="27" spans="1:12">
       <c r="B27" t="s">
         <v>20</v>
       </c>
@@ -1179,17 +1221,17 @@
         <v>79</v>
       </c>
     </row>
-    <row r="28" spans="1:7">
+    <row r="28" spans="1:12">
       <c r="B28" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="29" spans="1:7">
+    <row r="29" spans="1:12">
       <c r="B29" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="30" spans="1:7">
+    <row r="30" spans="1:12">
       <c r="A30">
         <v>7</v>
       </c>
@@ -1200,7 +1242,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="31" spans="1:7">
+    <row r="31" spans="1:12">
       <c r="A31">
         <v>8</v>
       </c>
@@ -1208,22 +1250,31 @@
         <v>49</v>
       </c>
       <c r="C31" s="2"/>
-    </row>
-    <row r="32" spans="1:7">
+      <c r="L31" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12">
       <c r="B32" t="s">
         <v>48</v>
       </c>
       <c r="C32" s="2"/>
-    </row>
-    <row r="33" spans="1:3">
+      <c r="L32" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12">
       <c r="A33">
         <v>9</v>
       </c>
       <c r="B33" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="34" spans="1:3">
+      <c r="L33" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12">
       <c r="A34">
         <v>10</v>
       </c>
@@ -1233,93 +1284,129 @@
       <c r="C34" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="35" spans="1:3">
+      <c r="L34" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="35" spans="1:12">
       <c r="A35">
         <v>11</v>
       </c>
       <c r="B35" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="36" spans="1:3">
+      <c r="L35" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="36" spans="1:12">
       <c r="A36">
         <v>12</v>
       </c>
       <c r="B36" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="37" spans="1:3">
+      <c r="L36" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="37" spans="1:12">
       <c r="A37">
         <v>13</v>
       </c>
       <c r="B37" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="38" spans="1:3">
+      <c r="L37" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="38" spans="1:12">
       <c r="A38">
         <v>14</v>
       </c>
       <c r="B38" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="39" spans="1:3">
+      <c r="L38" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="39" spans="1:12">
       <c r="A39">
         <v>15</v>
       </c>
       <c r="B39" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="40" spans="1:3">
+      <c r="L39" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="40" spans="1:12">
       <c r="A40">
         <v>16</v>
       </c>
       <c r="B40" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="41" spans="1:3">
+      <c r="L40" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="41" spans="1:12">
       <c r="A41">
         <v>17</v>
       </c>
       <c r="B41" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="42" spans="1:3">
+      <c r="L41" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="42" spans="1:12">
       <c r="A42">
         <v>18</v>
       </c>
       <c r="B42" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="43" spans="1:3">
+      <c r="L42" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="43" spans="1:12">
       <c r="B43" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="44" spans="1:3">
+      <c r="L43" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="44" spans="1:12">
       <c r="A44">
         <v>19</v>
       </c>
       <c r="B44" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="45" spans="1:3">
+      <c r="L44" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="45" spans="1:12">
       <c r="A45">
         <v>20</v>
       </c>
       <c r="B45" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="46" spans="1:3">
+      <c r="L45" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="46" spans="1:12">
       <c r="A46">
         <v>21</v>
       </c>
@@ -1327,7 +1414,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="47" spans="1:3">
+    <row r="47" spans="1:12">
       <c r="A47">
         <v>22</v>
       </c>
@@ -1335,7 +1422,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="48" spans="1:3">
+    <row r="48" spans="1:12">
       <c r="A48">
         <v>23</v>
       </c>
@@ -1409,8 +1496,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H20" sqref="H20"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I15" sqref="I15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1450,7 +1537,7 @@
         <v>43866</v>
       </c>
       <c r="B4">
-        <v>30</v>
+        <v>0.3</v>
       </c>
       <c r="C4" t="s">
         <v>85</v>

</xml_diff>